<commit_message>
Modified tables to include Descriptions
</commit_message>
<xml_diff>
--- a/data/2020-01-30.xlsx
+++ b/data/2020-01-30.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="80">
   <si>
     <t>DirectDebitPaymentRequestID</t>
   </si>
@@ -102,24 +102,12 @@
     <t>10000006</t>
   </si>
   <si>
-    <t>10000007</t>
-  </si>
-  <si>
-    <t>10000008</t>
-  </si>
-  <si>
-    <t>10000009</t>
-  </si>
-  <si>
     <t>10000013</t>
   </si>
   <si>
     <t>10000014</t>
   </si>
   <si>
-    <t>10000017</t>
-  </si>
-  <si>
     <t>10000018</t>
   </si>
   <si>
@@ -138,12 +126,6 @@
     <t>10000023</t>
   </si>
   <si>
-    <t>10000026</t>
-  </si>
-  <si>
-    <t>10000027</t>
-  </si>
-  <si>
     <t>10000028</t>
   </si>
   <si>
@@ -201,24 +183,6 @@
     <t>Young</t>
   </si>
   <si>
-    <t>Rob</t>
-  </si>
-  <si>
-    <t>Yalovsky</t>
-  </si>
-  <si>
-    <t>Gail</t>
-  </si>
-  <si>
-    <t>Wu</t>
-  </si>
-  <si>
-    <t>Jossef</t>
-  </si>
-  <si>
-    <t>Wright</t>
-  </si>
-  <si>
     <t>Michael</t>
   </si>
   <si>
@@ -231,9 +195,6 @@
     <t>Welcker</t>
   </si>
   <si>
-    <t>Wang</t>
-  </si>
-  <si>
     <t>Sharon</t>
   </si>
   <si>
@@ -268,15 +229,6 @@
   </si>
   <si>
     <t>Vanderhyde</t>
-  </si>
-  <si>
-    <t>Valdez</t>
-  </si>
-  <si>
-    <t>Jill</t>
-  </si>
-  <si>
-    <t>Uddin</t>
   </si>
   <si>
     <t>James</t>
@@ -730,7 +682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -738,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H26" sqref="A25:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,10 +740,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -850,10 +802,10 @@
         <v>520003</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -865,7 +817,7 @@
         <v>43858</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
@@ -912,10 +864,10 @@
         <v>201031</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -927,7 +879,7 @@
         <v>43857</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
@@ -974,10 +926,10 @@
         <v>523000</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -989,7 +941,7 @@
         <v>43856</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -1036,10 +988,10 @@
         <v>524000</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
@@ -1051,7 +1003,7 @@
         <v>43855</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -1098,10 +1050,10 @@
         <v>525000</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -1113,7 +1065,7 @@
         <v>43854</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
@@ -1160,10 +1112,10 @@
         <v>526000</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -1175,7 +1127,7 @@
         <v>43853</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M7" t="s">
         <v>18</v>
@@ -1204,7 +1156,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5234</v>
+        <v>5240</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -1213,31 +1165,31 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F8">
-        <v>527000</v>
+        <v>533000</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
       </c>
       <c r="J8" s="11">
-        <v>22.8</v>
+        <v>-64.8</v>
       </c>
       <c r="K8" s="6">
-        <v>43852</v>
+        <v>43846</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M8" t="s">
         <v>18</v>
@@ -1246,10 +1198,10 @@
         <v>18</v>
       </c>
       <c r="O8" s="8">
-        <v>43859</v>
+        <v>43865</v>
       </c>
       <c r="P8">
-        <v>1113</v>
+        <v>1107</v>
       </c>
       <c r="Q8" t="s">
         <v>18</v>
@@ -1261,12 +1213,12 @@
         <v>2</v>
       </c>
       <c r="T8" s="8">
-        <v>43863</v>
+        <v>43869</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5235</v>
+        <v>5241</v>
       </c>
       <c r="B9">
         <v>2020</v>
@@ -1275,31 +1227,31 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F9">
-        <v>528000</v>
+        <v>534000</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
       <c r="J9" s="11">
-        <v>8.1999999999999993</v>
+        <v>-79.400000000000006</v>
       </c>
       <c r="K9" s="6">
-        <v>43851</v>
+        <v>43845</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M9" t="s">
         <v>18</v>
@@ -1308,10 +1260,10 @@
         <v>18</v>
       </c>
       <c r="O9" s="8">
-        <v>43860</v>
+        <v>43866</v>
       </c>
       <c r="P9">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="Q9" t="s">
         <v>18</v>
@@ -1320,15 +1272,15 @@
         <v>8705</v>
       </c>
       <c r="S9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T9" s="8">
-        <v>43864</v>
+        <v>43870</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5236</v>
+        <v>5245</v>
       </c>
       <c r="B10">
         <v>2020</v>
@@ -1337,31 +1289,31 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F10">
-        <v>529000</v>
+        <v>538000</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="11">
-        <v>-6.4</v>
+        <v>-137.80000000000001</v>
       </c>
       <c r="K10" s="6">
-        <v>43850</v>
+        <v>43841</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M10" t="s">
         <v>18</v>
@@ -1370,10 +1322,10 @@
         <v>18</v>
       </c>
       <c r="O10" s="8">
-        <v>43861</v>
+        <v>43870</v>
       </c>
       <c r="P10">
-        <v>1111</v>
+        <v>1102</v>
       </c>
       <c r="Q10" t="s">
         <v>18</v>
@@ -1385,12 +1337,12 @@
         <v>2</v>
       </c>
       <c r="T10" s="8">
-        <v>43865</v>
+        <v>43874</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5240</v>
+        <v>5246</v>
       </c>
       <c r="B11">
         <v>2020</v>
@@ -1399,31 +1351,31 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F11">
-        <v>533000</v>
+        <v>539000</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
       </c>
       <c r="J11" s="11">
-        <v>-64.8</v>
+        <v>-152.4</v>
       </c>
       <c r="K11" s="6">
-        <v>43846</v>
+        <v>43840</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M11" t="s">
         <v>18</v>
@@ -1432,10 +1384,10 @@
         <v>18</v>
       </c>
       <c r="O11" s="8">
-        <v>43865</v>
+        <v>43871</v>
       </c>
       <c r="P11">
-        <v>1107</v>
+        <v>1101</v>
       </c>
       <c r="Q11" t="s">
         <v>18</v>
@@ -1444,15 +1396,15 @@
         <v>8705</v>
       </c>
       <c r="S11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T11" s="8">
-        <v>43869</v>
+        <v>43875</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5241</v>
+        <v>5247</v>
       </c>
       <c r="B12">
         <v>2020</v>
@@ -1461,31 +1413,31 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F12">
-        <v>534000</v>
+        <v>540000</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
         <v>18</v>
       </c>
       <c r="J12" s="11">
-        <v>-79.400000000000006</v>
+        <v>-167</v>
       </c>
       <c r="K12" s="6">
-        <v>43845</v>
+        <v>43839</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M12" t="s">
         <v>18</v>
@@ -1494,27 +1446,27 @@
         <v>18</v>
       </c>
       <c r="O12" s="8">
-        <v>43866</v>
+        <v>43872</v>
       </c>
       <c r="P12">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="Q12" t="s">
         <v>18</v>
       </c>
       <c r="R12">
-        <v>8705</v>
+        <v>8706</v>
       </c>
       <c r="S12">
         <v>1</v>
       </c>
       <c r="T12" s="8">
-        <v>43870</v>
+        <v>43876</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5244</v>
+        <v>5248</v>
       </c>
       <c r="B13">
         <v>2020</v>
@@ -1523,31 +1475,31 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F13">
-        <v>537000</v>
+        <v>541000</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="11">
-        <v>-123.2</v>
+        <v>-181.6</v>
       </c>
       <c r="K13" s="6">
-        <v>43842</v>
+        <v>43838</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="M13" t="s">
         <v>18</v>
@@ -1556,27 +1508,27 @@
         <v>18</v>
       </c>
       <c r="O13" s="8">
-        <v>43869</v>
+        <v>43873</v>
       </c>
       <c r="P13">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="Q13" t="s">
         <v>18</v>
       </c>
       <c r="R13">
-        <v>8705</v>
+        <v>8706</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13" s="8">
-        <v>43873</v>
+        <v>43877</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5245</v>
+        <v>5249</v>
       </c>
       <c r="B14">
         <v>2020</v>
@@ -1585,31 +1537,31 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F14">
-        <v>538000</v>
+        <v>542000</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="11">
-        <v>-137.80000000000001</v>
+        <v>-196.2</v>
       </c>
       <c r="K14" s="6">
-        <v>43841</v>
+        <v>43837</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="M14" t="s">
         <v>18</v>
@@ -1618,27 +1570,27 @@
         <v>18</v>
       </c>
       <c r="O14" s="8">
-        <v>43870</v>
+        <v>43874</v>
       </c>
       <c r="P14">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="Q14" t="s">
         <v>18</v>
       </c>
       <c r="R14">
-        <v>8705</v>
+        <v>8706</v>
       </c>
       <c r="S14">
         <v>2</v>
       </c>
       <c r="T14" s="8">
-        <v>43874</v>
+        <v>43878</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5246</v>
+        <v>5250</v>
       </c>
       <c r="B15">
         <v>2020</v>
@@ -1647,31 +1599,31 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F15">
-        <v>539000</v>
+        <v>543000</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
       </c>
       <c r="J15" s="11">
-        <v>-152.4</v>
+        <v>-210.8</v>
       </c>
       <c r="K15" s="6">
-        <v>43840</v>
+        <v>43836</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M15" t="s">
         <v>18</v>
@@ -1680,27 +1632,27 @@
         <v>18</v>
       </c>
       <c r="O15" s="8">
-        <v>43871</v>
+        <v>43875</v>
       </c>
       <c r="P15">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="Q15" t="s">
         <v>18</v>
       </c>
       <c r="R15">
-        <v>8705</v>
+        <v>8706</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T15" s="8">
-        <v>43875</v>
+        <v>43879</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5247</v>
+        <v>5255</v>
       </c>
       <c r="B16">
         <v>2020</v>
@@ -1709,31 +1661,31 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F16">
-        <v>540000</v>
+        <v>548000</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="11">
-        <v>-167</v>
+        <v>-283.8</v>
       </c>
       <c r="K16" s="6">
-        <v>43839</v>
+        <v>43831</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="M16" t="s">
         <v>18</v>
@@ -1742,10 +1694,10 @@
         <v>18</v>
       </c>
       <c r="O16" s="8">
-        <v>43872</v>
+        <v>43880</v>
       </c>
       <c r="P16">
-        <v>1100</v>
+        <v>1092</v>
       </c>
       <c r="Q16" t="s">
         <v>18</v>
@@ -1754,15 +1706,15 @@
         <v>8706</v>
       </c>
       <c r="S16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T16" s="8">
-        <v>43876</v>
+        <v>43884</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>5248</v>
+        <v>5256</v>
       </c>
       <c r="B17">
         <v>2020</v>
@@ -1771,31 +1723,31 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F17">
-        <v>541000</v>
+        <v>549000</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
       </c>
       <c r="J17" s="11">
-        <v>-181.6</v>
+        <v>-298.39999999999998</v>
       </c>
       <c r="K17" s="6">
-        <v>43838</v>
+        <v>43830</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M17" t="s">
         <v>18</v>
@@ -1804,10 +1756,10 @@
         <v>18</v>
       </c>
       <c r="O17" s="8">
-        <v>43873</v>
+        <v>43881</v>
       </c>
       <c r="P17">
-        <v>1099</v>
+        <v>1091</v>
       </c>
       <c r="Q17" t="s">
         <v>18</v>
@@ -1819,12 +1771,12 @@
         <v>2</v>
       </c>
       <c r="T17" s="8">
-        <v>43877</v>
+        <v>43885</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5249</v>
+        <v>5257</v>
       </c>
       <c r="B18">
         <v>2020</v>
@@ -1833,31 +1785,31 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F18">
-        <v>542000</v>
+        <v>550000</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="11">
-        <v>-196.2</v>
+        <v>-313</v>
       </c>
       <c r="K18" s="6">
-        <v>43837</v>
+        <v>43829</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
@@ -1866,10 +1818,10 @@
         <v>18</v>
       </c>
       <c r="O18" s="8">
-        <v>43874</v>
+        <v>43882</v>
       </c>
       <c r="P18">
-        <v>1098</v>
+        <v>1090</v>
       </c>
       <c r="Q18" t="s">
         <v>18</v>
@@ -1881,12 +1833,12 @@
         <v>2</v>
       </c>
       <c r="T18" s="8">
-        <v>43878</v>
+        <v>43886</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5250</v>
+        <v>5260</v>
       </c>
       <c r="B19">
         <v>2020</v>
@@ -1895,31 +1847,31 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F19">
-        <v>543000</v>
+        <v>553000</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="11">
-        <v>-210.8</v>
+        <v>-356.8</v>
       </c>
       <c r="K19" s="6">
-        <v>43836</v>
+        <v>43826</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="M19" t="s">
         <v>18</v>
@@ -1928,10 +1880,10 @@
         <v>18</v>
       </c>
       <c r="O19" s="8">
-        <v>43875</v>
+        <v>43885</v>
       </c>
       <c r="P19">
-        <v>1097</v>
+        <v>1087</v>
       </c>
       <c r="Q19" t="s">
         <v>18</v>
@@ -1943,12 +1895,12 @@
         <v>2</v>
       </c>
       <c r="T19" s="8">
-        <v>43879</v>
+        <v>43889</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5253</v>
+        <v>5261</v>
       </c>
       <c r="B20">
         <v>2020</v>
@@ -1957,31 +1909,31 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F20">
-        <v>546000</v>
+        <v>554000</v>
       </c>
       <c r="G20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" t="s">
         <v>77</v>
       </c>
-      <c r="H20" t="s">
-        <v>81</v>
-      </c>
       <c r="I20" t="s">
         <v>18</v>
       </c>
       <c r="J20" s="11">
-        <v>-254.6</v>
+        <v>-371.4</v>
       </c>
       <c r="K20" s="6">
-        <v>43833</v>
+        <v>43825</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="M20" t="s">
         <v>18</v>
@@ -1990,10 +1942,10 @@
         <v>18</v>
       </c>
       <c r="O20" s="8">
-        <v>43878</v>
+        <v>43886</v>
       </c>
       <c r="P20">
-        <v>1094</v>
+        <v>1086</v>
       </c>
       <c r="Q20" t="s">
         <v>18</v>
@@ -2002,381 +1954,9 @@
         <v>8706</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T20" s="8">
-        <v>43882</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5254</v>
-      </c>
-      <c r="B21">
-        <v>2020</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>13</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21">
-        <v>547000</v>
-      </c>
-      <c r="G21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H21" t="s">
-        <v>83</v>
-      </c>
-      <c r="I21" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="11">
-        <v>-269.2</v>
-      </c>
-      <c r="K21" s="6">
-        <v>43832</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M21" t="s">
-        <v>18</v>
-      </c>
-      <c r="N21" t="s">
-        <v>18</v>
-      </c>
-      <c r="O21" s="8">
-        <v>43879</v>
-      </c>
-      <c r="P21">
-        <v>1093</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>18</v>
-      </c>
-      <c r="R21">
-        <v>8706</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21" s="8">
-        <v>43883</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>5255</v>
-      </c>
-      <c r="B22">
-        <v>2020</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>14</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22">
-        <v>548000</v>
-      </c>
-      <c r="G22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" t="s">
-        <v>85</v>
-      </c>
-      <c r="I22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="11">
-        <v>-283.8</v>
-      </c>
-      <c r="K22" s="6">
-        <v>43831</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M22" t="s">
-        <v>18</v>
-      </c>
-      <c r="N22" t="s">
-        <v>18</v>
-      </c>
-      <c r="O22" s="8">
-        <v>43880</v>
-      </c>
-      <c r="P22">
-        <v>1092</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>18</v>
-      </c>
-      <c r="R22">
-        <v>8706</v>
-      </c>
-      <c r="S22">
-        <v>2</v>
-      </c>
-      <c r="T22" s="8">
-        <v>43884</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>5256</v>
-      </c>
-      <c r="B23">
-        <v>2020</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>15</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23">
-        <v>549000</v>
-      </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="11">
-        <v>-298.39999999999998</v>
-      </c>
-      <c r="K23" s="6">
-        <v>43830</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M23" t="s">
-        <v>18</v>
-      </c>
-      <c r="N23" t="s">
-        <v>18</v>
-      </c>
-      <c r="O23" s="8">
-        <v>43881</v>
-      </c>
-      <c r="P23">
-        <v>1091</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>18</v>
-      </c>
-      <c r="R23">
-        <v>8706</v>
-      </c>
-      <c r="S23">
-        <v>2</v>
-      </c>
-      <c r="T23" s="8">
-        <v>43885</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>5257</v>
-      </c>
-      <c r="B24">
-        <v>2020</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>16</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24">
-        <v>550000</v>
-      </c>
-      <c r="G24" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" t="s">
-        <v>89</v>
-      </c>
-      <c r="I24" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="11">
-        <v>-313</v>
-      </c>
-      <c r="K24" s="6">
-        <v>43829</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" t="s">
-        <v>18</v>
-      </c>
-      <c r="N24" t="s">
-        <v>18</v>
-      </c>
-      <c r="O24" s="8">
-        <v>43882</v>
-      </c>
-      <c r="P24">
-        <v>1090</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>18</v>
-      </c>
-      <c r="R24">
-        <v>8706</v>
-      </c>
-      <c r="S24">
-        <v>2</v>
-      </c>
-      <c r="T24" s="8">
-        <v>43886</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>5260</v>
-      </c>
-      <c r="B25">
-        <v>2020</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>19</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25">
-        <v>553000</v>
-      </c>
-      <c r="G25" t="s">
-        <v>90</v>
-      </c>
-      <c r="H25" t="s">
-        <v>91</v>
-      </c>
-      <c r="I25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" s="11">
-        <v>-356.8</v>
-      </c>
-      <c r="K25" s="6">
-        <v>43826</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M25" t="s">
-        <v>18</v>
-      </c>
-      <c r="N25" t="s">
-        <v>18</v>
-      </c>
-      <c r="O25" s="8">
-        <v>43885</v>
-      </c>
-      <c r="P25">
-        <v>1087</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>18</v>
-      </c>
-      <c r="R25">
-        <v>8706</v>
-      </c>
-      <c r="S25">
-        <v>2</v>
-      </c>
-      <c r="T25" s="8">
-        <v>43889</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>5261</v>
-      </c>
-      <c r="B26">
-        <v>2020</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>20</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26">
-        <v>554000</v>
-      </c>
-      <c r="G26" t="s">
-        <v>92</v>
-      </c>
-      <c r="H26" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="11">
-        <v>-371.4</v>
-      </c>
-      <c r="K26" s="6">
-        <v>43825</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M26" t="s">
-        <v>18</v>
-      </c>
-      <c r="N26" t="s">
-        <v>18</v>
-      </c>
-      <c r="O26" s="8">
-        <v>43886</v>
-      </c>
-      <c r="P26">
-        <v>1086</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>18</v>
-      </c>
-      <c r="R26">
-        <v>8706</v>
-      </c>
-      <c r="S26">
-        <v>2</v>
-      </c>
-      <c r="T26" s="8">
         <v>43890</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed implementation of results. Fixes Issue #1.
</commit_message>
<xml_diff>
--- a/data/2020-01-30.xlsx
+++ b/data/2020-01-30.xlsx
@@ -138,9 +138,6 @@
     <t>10000033</t>
   </si>
   <si>
-    <t>10000034</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>payeelastname</t>
+  </si>
+  <si>
+    <t>10000036</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +740,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -802,10 +802,10 @@
         <v>520003</v>
       </c>
       <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
         <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -817,7 +817,7 @@
         <v>43858</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
@@ -864,10 +864,10 @@
         <v>201031</v>
       </c>
       <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
         <v>43</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -879,7 +879,7 @@
         <v>43857</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
@@ -926,10 +926,10 @@
         <v>523000</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -941,7 +941,7 @@
         <v>43856</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -988,10 +988,10 @@
         <v>524000</v>
       </c>
       <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
@@ -1003,7 +1003,7 @@
         <v>43855</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -1050,10 +1050,10 @@
         <v>525000</v>
       </c>
       <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
         <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>49</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -1065,7 +1065,7 @@
         <v>43854</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
@@ -1112,10 +1112,10 @@
         <v>526000</v>
       </c>
       <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
         <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -1127,7 +1127,7 @@
         <v>43853</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M7" t="s">
         <v>18</v>
@@ -1174,10 +1174,10 @@
         <v>533000</v>
       </c>
       <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
         <v>52</v>
-      </c>
-      <c r="H8" t="s">
-        <v>53</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
@@ -1189,7 +1189,7 @@
         <v>43846</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M8" t="s">
         <v>18</v>
@@ -1236,10 +1236,10 @@
         <v>534000</v>
       </c>
       <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
         <v>54</v>
-      </c>
-      <c r="H9" t="s">
-        <v>55</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -1251,7 +1251,7 @@
         <v>43845</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" t="s">
         <v>18</v>
@@ -1298,10 +1298,10 @@
         <v>538000</v>
       </c>
       <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" t="s">
         <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
@@ -1313,7 +1313,7 @@
         <v>43841</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" t="s">
         <v>18</v>
@@ -1360,10 +1360,10 @@
         <v>539000</v>
       </c>
       <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
         <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>59</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
@@ -1375,7 +1375,7 @@
         <v>43840</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11" t="s">
         <v>18</v>
@@ -1422,10 +1422,10 @@
         <v>540000</v>
       </c>
       <c r="G12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" t="s">
         <v>60</v>
-      </c>
-      <c r="H12" t="s">
-        <v>61</v>
       </c>
       <c r="I12" t="s">
         <v>18</v>
@@ -1437,7 +1437,7 @@
         <v>43839</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M12" t="s">
         <v>18</v>
@@ -1484,10 +1484,10 @@
         <v>541000</v>
       </c>
       <c r="G13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
         <v>62</v>
-      </c>
-      <c r="H13" t="s">
-        <v>63</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
@@ -1499,7 +1499,7 @@
         <v>43838</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M13" t="s">
         <v>18</v>
@@ -1546,10 +1546,10 @@
         <v>542000</v>
       </c>
       <c r="G14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
         <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
@@ -1561,7 +1561,7 @@
         <v>43837</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M14" t="s">
         <v>18</v>
@@ -1608,10 +1608,10 @@
         <v>543000</v>
       </c>
       <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
         <v>66</v>
-      </c>
-      <c r="H15" t="s">
-        <v>67</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1623,7 +1623,7 @@
         <v>43836</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M15" t="s">
         <v>18</v>
@@ -1670,10 +1670,10 @@
         <v>548000</v>
       </c>
       <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
         <v>68</v>
-      </c>
-      <c r="H16" t="s">
-        <v>69</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1685,7 +1685,7 @@
         <v>43831</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" t="s">
         <v>18</v>
@@ -1732,10 +1732,10 @@
         <v>549000</v>
       </c>
       <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
         <v>70</v>
-      </c>
-      <c r="H17" t="s">
-        <v>71</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
@@ -1747,7 +1747,7 @@
         <v>43830</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M17" t="s">
         <v>18</v>
@@ -1794,10 +1794,10 @@
         <v>550000</v>
       </c>
       <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" t="s">
         <v>72</v>
-      </c>
-      <c r="H18" t="s">
-        <v>73</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
@@ -1809,7 +1809,7 @@
         <v>43829</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
@@ -1856,10 +1856,10 @@
         <v>553000</v>
       </c>
       <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
         <v>74</v>
-      </c>
-      <c r="H19" t="s">
-        <v>75</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
@@ -1871,7 +1871,7 @@
         <v>43826</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M19" t="s">
         <v>18</v>
@@ -1912,16 +1912,16 @@
         <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="F20">
         <v>554000</v>
       </c>
       <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
         <v>76</v>
-      </c>
-      <c r="H20" t="s">
-        <v>77</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
@@ -1933,7 +1933,7 @@
         <v>43825</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M20" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Changed implementation of results
</commit_message>
<xml_diff>
--- a/data/2020-01-30.xlsx
+++ b/data/2020-01-30.xlsx
@@ -138,9 +138,6 @@
     <t>10000033</t>
   </si>
   <si>
-    <t>10000034</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>payeelastname</t>
+  </si>
+  <si>
+    <t>10000036</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +740,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -802,10 +802,10 @@
         <v>520003</v>
       </c>
       <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
         <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -817,7 +817,7 @@
         <v>43858</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
@@ -864,10 +864,10 @@
         <v>201031</v>
       </c>
       <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
         <v>43</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -879,7 +879,7 @@
         <v>43857</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
@@ -926,10 +926,10 @@
         <v>523000</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -941,7 +941,7 @@
         <v>43856</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -988,10 +988,10 @@
         <v>524000</v>
       </c>
       <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
@@ -1003,7 +1003,7 @@
         <v>43855</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -1050,10 +1050,10 @@
         <v>525000</v>
       </c>
       <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
         <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>49</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -1065,7 +1065,7 @@
         <v>43854</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
@@ -1112,10 +1112,10 @@
         <v>526000</v>
       </c>
       <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
         <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -1127,7 +1127,7 @@
         <v>43853</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M7" t="s">
         <v>18</v>
@@ -1174,10 +1174,10 @@
         <v>533000</v>
       </c>
       <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
         <v>52</v>
-      </c>
-      <c r="H8" t="s">
-        <v>53</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
@@ -1189,7 +1189,7 @@
         <v>43846</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M8" t="s">
         <v>18</v>
@@ -1236,10 +1236,10 @@
         <v>534000</v>
       </c>
       <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
         <v>54</v>
-      </c>
-      <c r="H9" t="s">
-        <v>55</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -1251,7 +1251,7 @@
         <v>43845</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" t="s">
         <v>18</v>
@@ -1298,10 +1298,10 @@
         <v>538000</v>
       </c>
       <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" t="s">
         <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
@@ -1313,7 +1313,7 @@
         <v>43841</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" t="s">
         <v>18</v>
@@ -1360,10 +1360,10 @@
         <v>539000</v>
       </c>
       <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
         <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>59</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
@@ -1375,7 +1375,7 @@
         <v>43840</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11" t="s">
         <v>18</v>
@@ -1422,10 +1422,10 @@
         <v>540000</v>
       </c>
       <c r="G12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" t="s">
         <v>60</v>
-      </c>
-      <c r="H12" t="s">
-        <v>61</v>
       </c>
       <c r="I12" t="s">
         <v>18</v>
@@ -1437,7 +1437,7 @@
         <v>43839</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M12" t="s">
         <v>18</v>
@@ -1484,10 +1484,10 @@
         <v>541000</v>
       </c>
       <c r="G13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
         <v>62</v>
-      </c>
-      <c r="H13" t="s">
-        <v>63</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
@@ -1499,7 +1499,7 @@
         <v>43838</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M13" t="s">
         <v>18</v>
@@ -1546,10 +1546,10 @@
         <v>542000</v>
       </c>
       <c r="G14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
         <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
@@ -1561,7 +1561,7 @@
         <v>43837</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M14" t="s">
         <v>18</v>
@@ -1608,10 +1608,10 @@
         <v>543000</v>
       </c>
       <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
         <v>66</v>
-      </c>
-      <c r="H15" t="s">
-        <v>67</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1623,7 +1623,7 @@
         <v>43836</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M15" t="s">
         <v>18</v>
@@ -1670,10 +1670,10 @@
         <v>548000</v>
       </c>
       <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
         <v>68</v>
-      </c>
-      <c r="H16" t="s">
-        <v>69</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1685,7 +1685,7 @@
         <v>43831</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" t="s">
         <v>18</v>
@@ -1732,10 +1732,10 @@
         <v>549000</v>
       </c>
       <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
         <v>70</v>
-      </c>
-      <c r="H17" t="s">
-        <v>71</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
@@ -1747,7 +1747,7 @@
         <v>43830</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M17" t="s">
         <v>18</v>
@@ -1794,10 +1794,10 @@
         <v>550000</v>
       </c>
       <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" t="s">
         <v>72</v>
-      </c>
-      <c r="H18" t="s">
-        <v>73</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
@@ -1809,7 +1809,7 @@
         <v>43829</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
@@ -1856,10 +1856,10 @@
         <v>553000</v>
       </c>
       <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
         <v>74</v>
-      </c>
-      <c r="H19" t="s">
-        <v>75</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
@@ -1871,7 +1871,7 @@
         <v>43826</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M19" t="s">
         <v>18</v>
@@ -1912,16 +1912,16 @@
         <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="F20">
         <v>554000</v>
       </c>
       <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
         <v>76</v>
-      </c>
-      <c r="H20" t="s">
-        <v>77</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
@@ -1933,7 +1933,7 @@
         <v>43825</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M20" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Modified sample data files. Fixed #1
</commit_message>
<xml_diff>
--- a/data/2020-01-30.xlsx
+++ b/data/2020-01-30.xlsx
@@ -105,9 +105,6 @@
     <t>10000013</t>
   </si>
   <si>
-    <t>10000014</t>
-  </si>
-  <si>
     <t>10000018</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>10000036</t>
+  </si>
+  <si>
+    <t>10000040</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +740,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -802,10 +802,10 @@
         <v>520003</v>
       </c>
       <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
         <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -817,7 +817,7 @@
         <v>43858</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
@@ -864,10 +864,10 @@
         <v>201031</v>
       </c>
       <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
         <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -879,7 +879,7 @@
         <v>43857</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
@@ -926,10 +926,10 @@
         <v>523000</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -941,7 +941,7 @@
         <v>43856</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -988,10 +988,10 @@
         <v>524000</v>
       </c>
       <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
         <v>45</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
@@ -1003,7 +1003,7 @@
         <v>43855</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -1050,10 +1050,10 @@
         <v>525000</v>
       </c>
       <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
         <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>48</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -1065,7 +1065,7 @@
         <v>43854</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
@@ -1112,10 +1112,10 @@
         <v>526000</v>
       </c>
       <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
         <v>49</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -1127,7 +1127,7 @@
         <v>43853</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" t="s">
         <v>18</v>
@@ -1174,10 +1174,10 @@
         <v>533000</v>
       </c>
       <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
         <v>51</v>
-      </c>
-      <c r="H8" t="s">
-        <v>52</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
@@ -1189,7 +1189,7 @@
         <v>43846</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
         <v>18</v>
@@ -1230,16 +1230,16 @@
         <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="F9">
         <v>534000</v>
       </c>
       <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
         <v>53</v>
-      </c>
-      <c r="H9" t="s">
-        <v>54</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -1251,7 +1251,7 @@
         <v>43845</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" t="s">
         <v>18</v>
@@ -1292,16 +1292,16 @@
         <v>4</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>538000</v>
       </c>
       <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
         <v>55</v>
-      </c>
-      <c r="H10" t="s">
-        <v>56</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
@@ -1313,7 +1313,7 @@
         <v>43841</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" t="s">
         <v>18</v>
@@ -1354,16 +1354,16 @@
         <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>539000</v>
       </c>
       <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" t="s">
         <v>57</v>
-      </c>
-      <c r="H11" t="s">
-        <v>58</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
@@ -1375,7 +1375,7 @@
         <v>43840</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
         <v>18</v>
@@ -1416,16 +1416,16 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>540000</v>
       </c>
       <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
         <v>59</v>
-      </c>
-      <c r="H12" t="s">
-        <v>60</v>
       </c>
       <c r="I12" t="s">
         <v>18</v>
@@ -1437,7 +1437,7 @@
         <v>43839</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12" t="s">
         <v>18</v>
@@ -1478,16 +1478,16 @@
         <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13">
         <v>541000</v>
       </c>
       <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
         <v>61</v>
-      </c>
-      <c r="H13" t="s">
-        <v>62</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
@@ -1499,7 +1499,7 @@
         <v>43838</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M13" t="s">
         <v>18</v>
@@ -1540,16 +1540,16 @@
         <v>8</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14">
         <v>542000</v>
       </c>
       <c r="G14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" t="s">
         <v>63</v>
-      </c>
-      <c r="H14" t="s">
-        <v>64</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
@@ -1561,7 +1561,7 @@
         <v>43837</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M14" t="s">
         <v>18</v>
@@ -1602,16 +1602,16 @@
         <v>9</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15">
         <v>543000</v>
       </c>
       <c r="G15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
         <v>65</v>
-      </c>
-      <c r="H15" t="s">
-        <v>66</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1623,7 +1623,7 @@
         <v>43836</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M15" t="s">
         <v>18</v>
@@ -1664,16 +1664,16 @@
         <v>14</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16">
         <v>548000</v>
       </c>
       <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
         <v>67</v>
-      </c>
-      <c r="H16" t="s">
-        <v>68</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1685,7 +1685,7 @@
         <v>43831</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M16" t="s">
         <v>18</v>
@@ -1726,16 +1726,16 @@
         <v>15</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17">
         <v>549000</v>
       </c>
       <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
         <v>69</v>
-      </c>
-      <c r="H17" t="s">
-        <v>70</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
@@ -1747,7 +1747,7 @@
         <v>43830</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M17" t="s">
         <v>18</v>
@@ -1788,16 +1788,16 @@
         <v>16</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18">
         <v>550000</v>
       </c>
       <c r="G18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" t="s">
         <v>71</v>
-      </c>
-      <c r="H18" t="s">
-        <v>72</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
@@ -1809,7 +1809,7 @@
         <v>43829</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
@@ -1850,16 +1850,16 @@
         <v>19</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19">
         <v>553000</v>
       </c>
       <c r="G19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" t="s">
         <v>73</v>
-      </c>
-      <c r="H19" t="s">
-        <v>74</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
@@ -1871,7 +1871,7 @@
         <v>43826</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M19" t="s">
         <v>18</v>
@@ -1912,16 +1912,16 @@
         <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20">
         <v>554000</v>
       </c>
       <c r="G20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" t="s">
         <v>75</v>
-      </c>
-      <c r="H20" t="s">
-        <v>76</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
@@ -1933,7 +1933,7 @@
         <v>43825</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M20" t="s">
         <v>18</v>

</xml_diff>